<commit_message>
update test data to include ".0" test case
</commit_message>
<xml_diff>
--- a/tests/ExampleSTR.xlsx
+++ b/tests/ExampleSTR.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jandrews\Documents\GitHub\strprofiler\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EA58F8-DAAB-4CD9-B1B1-28B0D7A847DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4619004-C49F-4DED-ABC8-447014E09AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1463" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="144">
   <si>
     <t xml:space="preserve"> Sample Name</t>
   </si>
@@ -450,6 +450,9 @@
   </si>
   <si>
     <t xml:space="preserve"> PentaD</t>
+  </si>
+  <si>
+    <t>10.0</t>
   </si>
 </sst>
 </file>
@@ -967,10 +970,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1295,12 +1299,13 @@
   <dimension ref="A1:DG13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:111" x14ac:dyDescent="0.25">
@@ -1310,7 +1315,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -1645,7 +1650,7 @@
       <c r="B2" t="s">
         <v>139</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>16</v>
       </c>
       <c r="D2">
@@ -1980,7 +1985,7 @@
       <c r="B3" t="s">
         <v>140</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>11.3</v>
       </c>
       <c r="D3">
@@ -2315,7 +2320,7 @@
       <c r="B4" t="s">
         <v>141</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>12</v>
       </c>
       <c r="D4">
@@ -2650,7 +2655,7 @@
       <c r="B5" t="s">
         <v>131</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>9</v>
       </c>
       <c r="D5">
@@ -2985,7 +2990,7 @@
       <c r="B6" t="s">
         <v>124</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>11</v>
       </c>
       <c r="D6">
@@ -3320,7 +3325,7 @@
       <c r="B7" t="s">
         <v>134</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>135</v>
       </c>
       <c r="D7">
@@ -3655,7 +3660,7 @@
       <c r="B8" t="s">
         <v>134</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>135</v>
       </c>
       <c r="D8">
@@ -3990,8 +3995,8 @@
       <c r="B9" t="s">
         <v>124</v>
       </c>
-      <c r="C9">
-        <v>10</v>
+      <c r="C9" s="3" t="s">
+        <v>143</v>
       </c>
       <c r="D9">
         <v>392.89</v>
@@ -4325,7 +4330,7 @@
       <c r="B10" t="s">
         <v>139</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>12</v>
       </c>
       <c r="D10">
@@ -4660,7 +4665,7 @@
       <c r="B11" t="s">
         <v>140</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>20</v>
       </c>
       <c r="D11">
@@ -4995,7 +5000,7 @@
       <c r="B12" t="s">
         <v>141</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <v>10</v>
       </c>
       <c r="D12">
@@ -5330,7 +5335,7 @@
       <c r="B13" t="s">
         <v>142</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="3">
         <v>10</v>
       </c>
       <c r="D13">

</xml_diff>